<commit_message>
parsing various exports from fb-service, collecting per module code
</commit_message>
<xml_diff>
--- a/imi-lep-ws19.xlsx
+++ b/imi-lep-ws19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kleinen/mine/current/htw/studiengangssprecher/lehrplanung/19w/lehreinsatzplanungsparser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1870F3CE-747E-7A4F-97BE-B0C7BBBD7BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781C1151-44B5-C542-AF23-76542FB48732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32680" yWindow="-8760" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32600" yWindow="-6280" windowWidth="25600" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -971,8 +971,8 @@
   </sheetPr>
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>